<commit_message>
Addition of backend test
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_transfer_vtest.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_transfer_vtest.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="SampleTransferTemplate" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SampleTransfer" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Index" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -1240,7 +1240,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1287,13 +1287,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFBFBFBF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <i val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1312,7 +1305,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FFBFBFBF"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -1575,7 +1568,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1619,7 +1612,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1651,7 +1644,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1688,7 +1681,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFBFBFBF"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1746,7 +1739,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.67"/>
@@ -3808,7 +3801,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.33"/>

</xml_diff>